<commit_message>
Binary Tree Node Question
</commit_message>
<xml_diff>
--- a/SQL.xlsx
+++ b/SQL.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\first\SQL_Practice\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{606E97D8-8DA6-4E64-9E7F-365FA24D8ECC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA14247A-7E4C-4E41-8D68-84694C773712}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" xr2:uid="{44D32817-3C1B-4DB4-A46B-460F9BD46A84}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="105">
   <si>
     <t>Question</t>
   </si>
@@ -1727,6 +1727,36 @@
   </si>
   <si>
     <t>median</t>
+  </si>
+  <si>
+    <t>select h.hacker_id, h.name
+from Hackers h join Submissions sb on sb.hacker_id= h.hacker_id 
+join Challenges ch on ch.challenge_id= sb.challenge_id 
+join Difficulty df on df.difficulty_level= ch.difficulty_level</t>
+  </si>
+  <si>
+    <t>top competitior</t>
+  </si>
+  <si>
+    <t>SELECT DISTINCT(N), 
+IF(P IS NULL, 'Root', IF(N IN (SELECT P FROM BST), 'Inner', 'Leaf')) 
+FROM BST 
+ORDER BY N</t>
+  </si>
+  <si>
+    <t>select n , 
+case when p is null then 'Root' 
+when n not in (select p from BST where p is not null) then 'Leaf' 
+else 'Inner' 
+end as t 
+from BST 
+order by n asc</t>
+  </si>
+  <si>
+    <t>Print the type of nodein the binary tree (Root ,Leaf, Inner)</t>
+  </si>
+  <si>
+    <t>to do</t>
   </si>
 </sst>
 </file>
@@ -1822,7 +1852,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1835,21 +1865,9 @@
     <xf numFmtId="164" fontId="5" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="164" fontId="8" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2164,22 +2182,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7464BEF2-F22C-45E2-97C6-8B2A719DF0E6}">
-  <dimension ref="A1:E49"/>
+  <dimension ref="A1:E52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A41" workbookViewId="0">
-      <selection activeCell="A46" sqref="A46:B48"/>
+    <sheetView tabSelected="1" topLeftCell="A38" workbookViewId="0">
+      <selection activeCell="A52" sqref="A52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="111.7109375" style="10" customWidth="1"/>
+    <col min="1" max="1" width="111.7109375" style="1" customWidth="1"/>
     <col min="2" max="2" width="48.28515625" style="1" customWidth="1"/>
     <col min="3" max="3" width="10.42578125" style="5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
@@ -2189,8 +2207,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="30">
-      <c r="A2" s="10" t="s">
+    <row r="2" spans="1:4">
+      <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="1" t="s">
@@ -2200,8 +2218,8 @@
         <v>45019</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="30">
-      <c r="A3" s="10" t="s">
+    <row r="3" spans="1:4">
+      <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B3" s="1" t="s">
@@ -2212,7 +2230,7 @@
       </c>
     </row>
     <row r="4" spans="1:4">
-      <c r="A4" s="12" t="s">
+      <c r="A4" s="10" t="s">
         <v>6</v>
       </c>
       <c r="B4" s="1" t="s">
@@ -2223,7 +2241,7 @@
       </c>
     </row>
     <row r="5" spans="1:4">
-      <c r="A5" s="12" t="s">
+      <c r="A5" s="10" t="s">
         <v>8</v>
       </c>
       <c r="B5" s="1" t="s">
@@ -2234,7 +2252,7 @@
       </c>
     </row>
     <row r="6" spans="1:4">
-      <c r="A6" s="12" t="s">
+      <c r="A6" s="10" t="s">
         <v>10</v>
       </c>
       <c r="B6" s="1" t="s">
@@ -2245,7 +2263,7 @@
       </c>
     </row>
     <row r="7" spans="1:4">
-      <c r="A7" s="12" t="s">
+      <c r="A7" s="10" t="s">
         <v>13</v>
       </c>
       <c r="B7" s="2" t="s">
@@ -2256,7 +2274,7 @@
       </c>
     </row>
     <row r="8" spans="1:4">
-      <c r="A8" s="12" t="s">
+      <c r="A8" s="10" t="s">
         <v>15</v>
       </c>
       <c r="B8" s="1" t="s">
@@ -2266,8 +2284,8 @@
         <v>45020</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="29.25">
-      <c r="A9" s="13" t="s">
+    <row r="9" spans="1:4">
+      <c r="A9" s="11" t="s">
         <v>17</v>
       </c>
       <c r="B9" s="3" t="s">
@@ -2280,8 +2298,8 @@
         <v>25</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="30">
-      <c r="A10" s="13" t="s">
+    <row r="10" spans="1:4">
+      <c r="A10" s="11" t="s">
         <v>20</v>
       </c>
       <c r="B10" s="3" t="s">
@@ -2294,8 +2312,8 @@
         <v>25</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="29.25">
-      <c r="A11" s="14" t="s">
+    <row r="11" spans="1:4">
+      <c r="A11" s="12" t="s">
         <v>21</v>
       </c>
       <c r="B11" s="4" t="s">
@@ -2309,7 +2327,7 @@
       </c>
     </row>
     <row r="12" spans="1:4">
-      <c r="A12" s="11" t="s">
+      <c r="A12" s="4" t="s">
         <v>23</v>
       </c>
       <c r="B12" s="4" t="s">
@@ -2322,8 +2340,8 @@
         <v>33</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="30">
-      <c r="A13" s="14" t="s">
+    <row r="13" spans="1:4">
+      <c r="A13" s="12" t="s">
         <v>26</v>
       </c>
       <c r="B13" s="4" t="s">
@@ -2334,7 +2352,7 @@
       </c>
     </row>
     <row r="14" spans="1:4">
-      <c r="A14" s="12" t="s">
+      <c r="A14" s="10" t="s">
         <v>28</v>
       </c>
       <c r="B14" s="1" t="s">
@@ -2360,7 +2378,7 @@
       </c>
     </row>
     <row r="18" spans="1:3">
-      <c r="A18" s="10" t="s">
+      <c r="A18" s="1" t="s">
         <v>34</v>
       </c>
       <c r="B18" s="1" t="s">
@@ -2370,8 +2388,8 @@
         <v>45021</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="30">
-      <c r="A19" s="12" t="s">
+    <row r="19" spans="1:3">
+      <c r="A19" s="10" t="s">
         <v>36</v>
       </c>
       <c r="B19" s="1" t="s">
@@ -2381,8 +2399,8 @@
         <v>45021</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="30">
-      <c r="A20" s="12" t="s">
+    <row r="20" spans="1:3">
+      <c r="A20" s="10" t="s">
         <v>38</v>
       </c>
       <c r="B20" s="1" t="s">
@@ -2392,8 +2410,8 @@
         <v>45021</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="44.25">
-      <c r="A21" s="14" t="s">
+    <row r="21" spans="1:3">
+      <c r="A21" s="12" t="s">
         <v>41</v>
       </c>
       <c r="B21" s="4" t="s">
@@ -2403,8 +2421,8 @@
         <v>45022</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="30">
-      <c r="A22" s="12" t="s">
+    <row r="22" spans="1:3">
+      <c r="A22" s="10" t="s">
         <v>42</v>
       </c>
       <c r="B22" s="1" t="s">
@@ -2414,8 +2432,8 @@
         <v>45022</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="44.25">
-      <c r="A23" s="12" t="s">
+    <row r="23" spans="1:3">
+      <c r="A23" s="10" t="s">
         <v>44</v>
       </c>
       <c r="B23" s="1" t="s">
@@ -2426,7 +2444,7 @@
       </c>
     </row>
     <row r="24" spans="1:3">
-      <c r="A24" s="14" t="s">
+      <c r="A24" s="12" t="s">
         <v>46</v>
       </c>
       <c r="B24" s="4" t="s">
@@ -2437,7 +2455,7 @@
       </c>
     </row>
     <row r="25" spans="1:3">
-      <c r="A25" s="12" t="s">
+      <c r="A25" s="10" t="s">
         <v>48</v>
       </c>
       <c r="B25" s="1" t="s">
@@ -2448,7 +2466,7 @@
       </c>
     </row>
     <row r="26" spans="1:3">
-      <c r="A26" s="12" t="s">
+      <c r="A26" s="10" t="s">
         <v>51</v>
       </c>
       <c r="B26" s="1" t="s">
@@ -2459,7 +2477,7 @@
       </c>
     </row>
     <row r="27" spans="1:3">
-      <c r="A27" s="12" t="s">
+      <c r="A27" s="10" t="s">
         <v>52</v>
       </c>
       <c r="B27" s="1" t="s">
@@ -2470,7 +2488,7 @@
       </c>
     </row>
     <row r="28" spans="1:3">
-      <c r="A28" s="12" t="s">
+      <c r="A28" s="10" t="s">
         <v>55</v>
       </c>
       <c r="B28" s="1" t="s">
@@ -2481,7 +2499,7 @@
       </c>
     </row>
     <row r="29" spans="1:3">
-      <c r="A29" s="12" t="s">
+      <c r="A29" s="10" t="s">
         <v>56</v>
       </c>
       <c r="B29" s="1" t="s">
@@ -2492,7 +2510,7 @@
       </c>
     </row>
     <row r="30" spans="1:3">
-      <c r="A30" s="12" t="s">
+      <c r="A30" s="10" t="s">
         <v>58</v>
       </c>
       <c r="B30" s="3" t="s">
@@ -2502,8 +2520,8 @@
         <v>45022</v>
       </c>
     </row>
-    <row r="31" spans="1:3" ht="29.25">
-      <c r="A31" s="14" t="s">
+    <row r="31" spans="1:3">
+      <c r="A31" s="12" t="s">
         <v>61</v>
       </c>
       <c r="B31" s="4" t="s">
@@ -2513,8 +2531,8 @@
         <v>45022</v>
       </c>
     </row>
-    <row r="32" spans="1:3" ht="60">
-      <c r="A32" s="11" t="s">
+    <row r="32" spans="1:3">
+      <c r="A32" s="4" t="s">
         <v>62</v>
       </c>
       <c r="B32" s="4" t="s">
@@ -2524,8 +2542,8 @@
         <v>45022</v>
       </c>
     </row>
-    <row r="33" spans="1:5" ht="29.25">
-      <c r="A33" s="12" t="s">
+    <row r="33" spans="1:5">
+      <c r="A33" s="10" t="s">
         <v>64</v>
       </c>
       <c r="B33" s="1" t="s">
@@ -2535,8 +2553,8 @@
         <v>45022</v>
       </c>
     </row>
-    <row r="34" spans="1:5" ht="58.5">
-      <c r="A34" s="14" t="s">
+    <row r="34" spans="1:5">
+      <c r="A34" s="12" t="s">
         <v>67</v>
       </c>
       <c r="B34" s="4" t="s">
@@ -2552,8 +2570,8 @@
       </c>
       <c r="C35" s="8"/>
     </row>
-    <row r="36" spans="1:5" ht="29.25">
-      <c r="A36" s="12" t="s">
+    <row r="36" spans="1:5">
+      <c r="A36" s="10" t="s">
         <v>69</v>
       </c>
       <c r="B36" s="1" t="s">
@@ -2563,8 +2581,8 @@
         <v>45022</v>
       </c>
     </row>
-    <row r="37" spans="1:5" ht="29.25">
-      <c r="A37" s="14" t="s">
+    <row r="37" spans="1:5">
+      <c r="A37" s="12" t="s">
         <v>71</v>
       </c>
       <c r="B37" s="4" t="s">
@@ -2574,8 +2592,8 @@
         <v>45022</v>
       </c>
     </row>
-    <row r="38" spans="1:5" ht="29.25">
-      <c r="A38" s="14" t="s">
+    <row r="38" spans="1:5">
+      <c r="A38" s="12" t="s">
         <v>73</v>
       </c>
       <c r="B38" s="4" t="s">
@@ -2585,8 +2603,8 @@
         <v>45023</v>
       </c>
     </row>
-    <row r="39" spans="1:5" ht="29.25">
-      <c r="A39" s="12" t="s">
+    <row r="39" spans="1:5">
+      <c r="A39" s="10" t="s">
         <v>75</v>
       </c>
       <c r="B39" s="1" t="s">
@@ -2597,7 +2615,7 @@
       </c>
     </row>
     <row r="40" spans="1:5">
-      <c r="A40" s="14" t="s">
+      <c r="A40" s="12" t="s">
         <v>77</v>
       </c>
       <c r="B40" s="4" t="s">
@@ -2611,7 +2629,7 @@
       </c>
     </row>
     <row r="41" spans="1:5">
-      <c r="A41" s="14" t="s">
+      <c r="A41" s="12" t="s">
         <v>79</v>
       </c>
       <c r="B41" s="4" t="s">
@@ -2624,8 +2642,8 @@
         <v>83</v>
       </c>
     </row>
-    <row r="42" spans="1:5" ht="30">
-      <c r="A42" s="14" t="s">
+    <row r="42" spans="1:5">
+      <c r="A42" s="12" t="s">
         <v>81</v>
       </c>
       <c r="B42" s="4" t="s">
@@ -2639,7 +2657,7 @@
       </c>
     </row>
     <row r="43" spans="1:5">
-      <c r="A43" s="14" t="s">
+      <c r="A43" s="12" t="s">
         <v>87</v>
       </c>
       <c r="B43" s="1" t="s">
@@ -2653,7 +2671,7 @@
       </c>
     </row>
     <row r="44" spans="1:5">
-      <c r="A44" s="14" t="s">
+      <c r="A44" s="12" t="s">
         <v>86</v>
       </c>
       <c r="B44" s="1" t="s">
@@ -2670,7 +2688,7 @@
       </c>
     </row>
     <row r="45" spans="1:5">
-      <c r="A45" s="14" t="s">
+      <c r="A45" s="12" t="s">
         <v>88</v>
       </c>
       <c r="B45" s="1" t="s">
@@ -2686,8 +2704,8 @@
         <v>91</v>
       </c>
     </row>
-    <row r="46" spans="1:5" ht="43.5">
-      <c r="A46" s="14" t="s">
+    <row r="46" spans="1:5">
+      <c r="A46" s="12" t="s">
         <v>92</v>
       </c>
       <c r="B46" s="1" t="s">
@@ -2697,8 +2715,8 @@
         <v>45024</v>
       </c>
     </row>
-    <row r="47" spans="1:5" ht="43.5">
-      <c r="A47" s="12" t="s">
+    <row r="47" spans="1:5">
+      <c r="A47" s="10" t="s">
         <v>95</v>
       </c>
       <c r="B47" s="1" t="s">
@@ -2712,13 +2730,55 @@
       <c r="B48" s="1" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="49" spans="1:2" ht="75">
-      <c r="A49" s="10" t="s">
+      <c r="C48" s="9">
+        <v>45024</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4">
+      <c r="A49" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="B49" s="10" t="s">
+      <c r="B49" s="1" t="s">
         <v>97</v>
+      </c>
+      <c r="C49" s="9">
+        <v>45024</v>
+      </c>
+      <c r="D49" s="1" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4">
+      <c r="A50" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="C50" s="9">
+        <v>45025</v>
+      </c>
+      <c r="D50" s="1" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4">
+      <c r="A51" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="C51" s="9">
+        <v>45027</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4">
+      <c r="B52" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="C52" s="9">
+        <v>45027</v>
       </c>
     </row>
   </sheetData>

</xml_diff>